<commit_message>
19 20 21 课
</commit_message>
<xml_diff>
--- a/Excel/StartSceneConfig@s.xlsx
+++ b/Excel/StartSceneConfig@s.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UnityWorkSpace\ET-EUI_Acrsm\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AF09666-7B4B-434B-8FD0-F6A987A33987}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03D7821C-7EC4-4735-B8AE-291F4B19AACC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="26">
   <si>
     <t>Id</t>
   </si>
@@ -93,6 +93,13 @@
   </si>
   <si>
     <t>Account</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>LoginCenter</t>
+  </si>
+  <si>
+    <t>LoginCenter</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -484,10 +491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C3:H12"/>
+  <dimension ref="C3:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.3"/>
@@ -692,6 +699,23 @@
       </c>
       <c r="H12" s="3">
         <v>10005</v>
+      </c>
+    </row>
+    <row r="13" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C13" s="3">
+        <v>8</v>
+      </c>
+      <c r="D13" s="3">
+        <v>1</v>
+      </c>
+      <c r="E13" s="3">
+        <v>1</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>